<commit_message>
:white_check_mark: ROUTE 10:  implemented Integration test to get user.
</commit_message>
<xml_diff>
--- a/Sample Test Case.xlsx
+++ b/Sample Test Case.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -48,7 +48,7 @@
 3. Check if token exists in body and token is composed of 3 parts.</t>
   </si>
   <si>
-    <t>Post successful creation check</t>
+    <t>ROUTE 5: POST Successful creation of post by authenticated user</t>
   </si>
   <si>
     <t>api/posts/</t>
@@ -63,6 +63,34 @@
     <t>1. Send a post request with the required fields: Title, Description, valid jwt token.
 2. Check response field according to requirements.
 3. Cross validated the resposne field value with that in the database table</t>
+  </si>
+  <si>
+    <t>ROUTE 10: GET request post made an authenticated user</t>
+  </si>
+  <si>
+    <t>/api/posts/{:id}</t>
+  </si>
+  <si>
+    <t>To check if user post is getting returned when requested by authenticated user who created it.</t>
+  </si>
+  <si>
+    <t>1. Send a GET request with JWT in header.
+2. Check headers to authenticate user.
+3. Check if userid is valid and return post made by that user whose database id is given in params.</t>
+  </si>
+  <si>
+    <t>ROUTE 11: GET  request all posts created by an authenticated user</t>
+  </si>
+  <si>
+    <t>/api/all_posts</t>
+  </si>
+  <si>
+    <t>To check if all the posts created by used is being sent when requested</t>
+  </si>
+  <si>
+    <t>1. Send a GET request with JWT in header.
+2. Check headers to authenticate user.
+3. Check if userid is valid and return all posts made by that user.</t>
   </si>
   <si>
     <t>Post creation with Title field missing</t>
@@ -82,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,7 +120,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -100,6 +128,12 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -131,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -147,6 +181,12 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
@@ -465,17 +505,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="66.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="37.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="23.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="29.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="66.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -495,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="58.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="47.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -512,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="72">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="75">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -534,16 +574,50 @@
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="58.5">
+      <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="58.5">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:white_check_mark: implement Integration test for ROUTE 9
</commit_message>
<xml_diff>
--- a/Sample Test Case.xlsx
+++ b/Sample Test Case.xlsx
@@ -48,21 +48,32 @@
 3. Check if token exists in body and token is composed of 3 parts.</t>
   </si>
   <si>
-    <t>ROUTE 5: POST Successful creation of post by authenticated user</t>
-  </si>
-  <si>
-    <t>api/posts/</t>
-  </si>
-  <si>
-    <t>To check if the post is getting created by providing all the required parameters with correct format</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>1. Send a post request with the required fields: Title, Description, valid jwt token.
-2. Check response field according to requirements.
-3. Cross validated the resposne field value with that in the database table</t>
+    <t>ROUTE 4: GET Request user profile</t>
+  </si>
+  <si>
+    <t>/api/user</t>
+  </si>
+  <si>
+    <t>To check if user profile is sent in res body</t>
+  </si>
+  <si>
+    <t>1. Send a GET request with JWT in header.
+2. Check headers to authenticate user.
+3. Check if userid is valid and return user details of that user whose database id is given in params.</t>
+  </si>
+  <si>
+    <t>ROUTE 9: POST add new comment to an existing post</t>
+  </si>
+  <si>
+    <t>/api/comment/{:id}</t>
+  </si>
+  <si>
+    <t>To check if comments gets added in the post object</t>
+  </si>
+  <si>
+    <t>1. Send a post request with the required field: comment and JWT in headers.
+2. If post with id exists, add comment to post object after saving the comment in comment database.
+3. Send the comment id and success message as response.</t>
   </si>
   <si>
     <t>ROUTE 10: GET request post made an authenticated user</t>
@@ -91,18 +102,6 @@
     <t>1. Send a GET request with JWT in header.
 2. Check headers to authenticate user.
 3. Check if userid is valid and return all posts made by that user.</t>
-  </si>
-  <si>
-    <t>Post creation with Title field missing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To check if the post creation is unsucessfull if Title field is miising in the POST request </t>
-  </si>
-  <si>
-    <t>1. Check in database for the number of posts for the test user.
-2. Send a POST request with Title field missing.
-3. Check the resposne field according to requirement.
-4. Check in database if no new post is created for the user.</t>
   </si>
 </sst>
 </file>
@@ -165,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -182,17 +181,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
@@ -511,11 +507,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="66.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="37.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="23.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="29.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="66.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -552,68 +548,68 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="75">
-      <c r="A3" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="58.5">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="64.5">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="58.5">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
+      <c r="E4" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="58.5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="58.5">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="8" t="s">

</xml_diff>